<commit_message>
Solve the problem that the content is "null"
</commit_message>
<xml_diff>
--- a/src/test/resources/normalNoTitle.xlsx
+++ b/src/test/resources/normalNoTitle.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maqiang/workspace/private/ProteanBear/PbPOITemplate/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3282B18F-7161-2746-8F1D-EC1A003421BA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>你好</t>
     <rPh sb="0" eb="1">
@@ -37,16 +38,21 @@
   </si>
   <si>
     <t>测试</t>
-    <rPh sb="0" eb="1">
-      <t>ce'shi</t>
-    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发的发的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="177" formatCode="yyyy/m/d\ h:mm;@"/>
@@ -88,11 +94,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -102,6 +109,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -369,11 +379,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -381,6 +391,7 @@
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="23.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -396,8 +407,8 @@
       <c r="D1" s="3">
         <v>43005.431944444441</v>
       </c>
-      <c r="E1">
-        <v>1</v>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -413,8 +424,8 @@
       <c r="D2" s="3">
         <v>43005.433333333334</v>
       </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>